<commit_message>
ajustando etiqueta e trocando nome lote sap por lot
</commit_message>
<xml_diff>
--- a/BLOQUEADO.xlsx
+++ b/BLOQUEADO.xlsx
@@ -257,9 +257,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1596600</xdr:colOff>
+      <xdr:colOff>1596240</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>37800</xdr:rowOff>
+      <xdr:rowOff>37440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -272,8 +272,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6210360" y="5486400"/>
-          <a:ext cx="1837800" cy="1790280"/>
+          <a:off x="6211080" y="5486400"/>
+          <a:ext cx="1837800" cy="1789920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -297,7 +297,7 @@
   <dimension ref="A1:F121"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="true" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -375,9 +375,7 @@
       <c r="F8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="n">
-        <v>944872</v>
-      </c>
+      <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
@@ -432,7 +430,7 @@
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
-      <c r="F15" s="8"/>
+      <c r="F15" s="7"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="7"/>
@@ -440,7 +438,7 @@
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
-      <c r="F16" s="8"/>
+      <c r="F16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="107.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="7"/>
@@ -448,7 +446,7 @@
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
-      <c r="F17" s="8"/>
+      <c r="F17" s="7"/>
     </row>
     <row r="18" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="9"/>

</xml_diff>